<commit_message>
add 11.2 sheet average use and amout
</commit_message>
<xml_diff>
--- a/storage/excel/sum11_1.xlsx
+++ b/storage/excel/sum11_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>บทที่ 11 ข้อมูลแหล่งพลังงาน</t>
   </si>
@@ -104,18 +104,6 @@
     <t>ฟืน</t>
   </si>
   <si>
-    <t>no_ra800_o81_ti801_ch802_o266_ra803(221)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o266_ra803(222)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o266_ra803(223)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o266_ra803(224)</t>
-  </si>
-  <si>
     <t>ค่าเฉลี่ย</t>
   </si>
   <si>
@@ -125,31 +113,7 @@
     <t>ถ่าน</t>
   </si>
   <si>
-    <t>no_ra800_o81_ti801_ch802_o267_ra803(221)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o267_ra803(222)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o267_ra803(223)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o267_ra803(224)</t>
-  </si>
-  <si>
     <t>แกลบ</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o268_ra803(221)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o268_ra803(222)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o268_ra803(223)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o268_ra803(224)</t>
   </si>
   <si>
     <t xml:space="preserve">  ขนส่งโดยไม่ใช้เชื้อเพลิง</t>
@@ -158,34 +122,10 @@
     <t>วัสดุเหลือใช้ทางการเกษตร</t>
   </si>
   <si>
-    <t>no_ra800_o81_ti801_ch802_o269_ra803(221)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o269_ra803(222)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o269_ra803(223)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o269_ra803(224)</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ขนส่งโดยใช้เชื้อเพลิง</t>
   </si>
   <si>
     <t>อื่นๆ</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o1_ra803(221)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o1_ra803(222)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o1_ra803(223)</t>
-  </si>
-  <si>
-    <t>no_ra800_o81_ti801_ch802_o1_ra803(224)</t>
   </si>
   <si>
     <t>-</t>
@@ -2013,133 +1953,109 @@
       <c r="AF10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AG10" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="AG10" s="12"/>
       <c r="AH10" s="12"/>
-      <c r="AI10" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="AI10" s="12"/>
       <c r="AJ10" s="12"/>
-      <c r="AK10" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="AK10" s="12"/>
       <c r="AL10" s="12"/>
-      <c r="AM10" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="AM10" s="12"/>
       <c r="AN10" s="12"/>
       <c r="AP10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AQ10" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="AQ10" s="12"/>
       <c r="AR10" s="12"/>
-      <c r="AS10" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="AS10" s="12"/>
       <c r="AT10" s="12"/>
-      <c r="AU10" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="AU10" s="12"/>
       <c r="AV10" s="12"/>
-      <c r="AW10" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="AW10" s="12"/>
       <c r="AX10" s="12"/>
       <c r="AZ10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="BA10" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="BA10" s="12"/>
       <c r="BB10" s="12"/>
-      <c r="BC10" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="BC10" s="12"/>
       <c r="BD10" s="12"/>
-      <c r="BE10" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="BE10" s="12"/>
       <c r="BF10" s="12"/>
-      <c r="BG10" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="BG10" s="12"/>
       <c r="BH10" s="12"/>
       <c r="BJ10" s="32"/>
       <c r="BK10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BL10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BM10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BN10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BO10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BP10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BQ10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BR10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BS10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BT10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BU10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BV10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="BX10" s="32"/>
       <c r="BY10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="BZ10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="CA10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="CB10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="CC10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="CD10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="CE10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="CF10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="CG10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="CH10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="CI10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="CJ10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="CL10" s="43"/>
       <c r="CM10" s="20" t="s">
@@ -2180,45 +2096,45 @@
       </c>
       <c r="CZ10" s="32"/>
       <c r="DA10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="DB10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="DC10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="DD10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="DE10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="DF10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="DG10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="DH10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="DI10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="DJ10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="DK10" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="DL10" s="18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:116">
       <c r="B11" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="52">
         <v>116113.95097772</v>
@@ -2245,7 +2161,7 @@
         <v>0.040022654867257</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M11" s="52">
         <v>16853.070088289</v>
@@ -2272,7 +2188,7 @@
         <v>0.11911504424779</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="W11" s="52">
         <v>101108.20987274</v>
@@ -2299,61 +2215,37 @@
         <v>0</v>
       </c>
       <c r="AF11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG11" s="12" t="s">
-        <v>36</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="AG11" s="12"/>
       <c r="AH11" s="12"/>
-      <c r="AI11" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="AI11" s="12"/>
       <c r="AJ11" s="12"/>
-      <c r="AK11" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="AK11" s="12"/>
       <c r="AL11" s="12"/>
-      <c r="AM11" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="AM11" s="12"/>
       <c r="AN11" s="12"/>
       <c r="AP11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ11" s="12" t="s">
-        <v>36</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="AQ11" s="12"/>
       <c r="AR11" s="12"/>
-      <c r="AS11" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="AS11" s="12"/>
       <c r="AT11" s="12"/>
-      <c r="AU11" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="AU11" s="12"/>
       <c r="AV11" s="12"/>
-      <c r="AW11" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="AW11" s="12"/>
       <c r="AX11" s="12"/>
       <c r="AZ11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="BA11" s="12" t="s">
-        <v>36</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="BA11" s="12"/>
       <c r="BB11" s="12"/>
-      <c r="BC11" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="BC11" s="12"/>
       <c r="BD11" s="12"/>
-      <c r="BE11" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="BE11" s="12"/>
       <c r="BF11" s="12"/>
-      <c r="BG11" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="BG11" s="12"/>
       <c r="BH11" s="12"/>
       <c r="BJ11" s="7" t="s">
         <v>28</v>
@@ -2386,22 +2278,22 @@
         <v>28</v>
       </c>
       <c r="BY11" s="52">
-        <v>168.67148809524</v>
+        <v>427.92761446886</v>
       </c>
       <c r="BZ11" s="52">
-        <v>6.409845121061</v>
+        <v>9.8910614982318</v>
       </c>
       <c r="CA11" s="52">
-        <v>133.24978981582</v>
+        <v>547.02078223185</v>
       </c>
       <c r="CB11" s="52">
-        <v>0.058757021013123</v>
+        <v>0.68973599461653</v>
       </c>
       <c r="CC11" s="52">
-        <v>150.96063895553</v>
+        <v>487.47419835036</v>
       </c>
       <c r="CD11" s="52">
-        <v>3.2343010710371</v>
+        <v>5.2903987464242</v>
       </c>
       <c r="CE11" s="12"/>
       <c r="CF11" s="12"/>
@@ -2454,7 +2346,7 @@
     </row>
     <row r="12" spans="1:116">
       <c r="B12" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C12" s="52">
         <v>1784.8038156153</v>
@@ -2481,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="M12" s="52">
         <v>0</v>
@@ -2508,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="W12" s="52">
         <v>1837.2526066584</v>
@@ -2535,64 +2427,40 @@
         <v>0</v>
       </c>
       <c r="AF12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG12" s="12" t="s">
-        <v>41</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="AG12" s="12"/>
       <c r="AH12" s="12"/>
-      <c r="AI12" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="AI12" s="12"/>
       <c r="AJ12" s="12"/>
-      <c r="AK12" s="12" t="s">
-        <v>43</v>
-      </c>
+      <c r="AK12" s="12"/>
       <c r="AL12" s="12"/>
-      <c r="AM12" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="AM12" s="12"/>
       <c r="AN12" s="12"/>
       <c r="AP12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ12" s="12" t="s">
-        <v>41</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="AQ12" s="12"/>
       <c r="AR12" s="12"/>
-      <c r="AS12" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="AS12" s="12"/>
       <c r="AT12" s="12"/>
-      <c r="AU12" s="12" t="s">
-        <v>43</v>
-      </c>
+      <c r="AU12" s="12"/>
       <c r="AV12" s="12"/>
-      <c r="AW12" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="AW12" s="12"/>
       <c r="AX12" s="12"/>
       <c r="AZ12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="BA12" s="12" t="s">
-        <v>41</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="BA12" s="12"/>
       <c r="BB12" s="12"/>
-      <c r="BC12" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="BC12" s="12"/>
       <c r="BD12" s="12"/>
-      <c r="BE12" s="12" t="s">
-        <v>43</v>
-      </c>
+      <c r="BE12" s="12"/>
       <c r="BF12" s="12"/>
-      <c r="BG12" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="BG12" s="12"/>
       <c r="BH12" s="12"/>
       <c r="BJ12" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BK12" s="53">
         <v>57.111032967033</v>
@@ -2619,25 +2487,25 @@
       <c r="BU12" s="12"/>
       <c r="BV12" s="12"/>
       <c r="BX12" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BY12" s="52">
-        <v>31.388</v>
+        <v>260.89925274725</v>
       </c>
       <c r="BZ12" s="52">
-        <v>4.8332335429462</v>
+        <v>20.216689159951</v>
       </c>
       <c r="CA12" s="52">
-        <v>104.87366122449</v>
+        <v>319.41884897959</v>
       </c>
       <c r="CB12" s="52">
-        <v>1.0779164941799</v>
+        <v>4.2570780266762</v>
       </c>
       <c r="CC12" s="52">
-        <v>68.130830612245</v>
+        <v>290.15905086342</v>
       </c>
       <c r="CD12" s="52">
-        <v>2.9555750185631</v>
+        <v>12.236883593314</v>
       </c>
       <c r="CE12" s="12"/>
       <c r="CF12" s="12"/>
@@ -2646,25 +2514,25 @@
       <c r="CI12" s="12"/>
       <c r="CJ12" s="12"/>
       <c r="CL12" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="CM12" s="52">
         <v>77480.924720096</v>
       </c>
       <c r="CN12" s="52">
-        <v>0.054804321426264</v>
+        <v>5.4804321426264</v>
       </c>
       <c r="CO12" s="52">
         <v>457669.1560631</v>
       </c>
       <c r="CP12" s="52">
-        <v>0.14989313411184</v>
+        <v>14.989313411184</v>
       </c>
       <c r="CQ12" s="52">
         <v>526861.77168563</v>
       </c>
       <c r="CR12" s="52">
-        <v>0.11794329304949</v>
+        <v>11.794329304949</v>
       </c>
       <c r="CS12" s="12"/>
       <c r="CT12" s="12"/>
@@ -2673,7 +2541,7 @@
       <c r="CW12" s="12"/>
       <c r="CX12" s="12"/>
       <c r="CZ12" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="DA12" s="52">
         <v>27.961022527473</v>
@@ -2702,7 +2570,7 @@
     </row>
     <row r="13" spans="1:116">
       <c r="B13" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C13" s="52">
         <v>0</v>
@@ -2729,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="M13" s="52">
         <v>0</v>
@@ -2756,7 +2624,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="W13" s="52">
         <v>0</v>
@@ -2783,64 +2651,40 @@
         <v>0</v>
       </c>
       <c r="AF13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG13" s="12" t="s">
-        <v>47</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="AG13" s="12"/>
       <c r="AH13" s="12"/>
-      <c r="AI13" s="12" t="s">
-        <v>48</v>
-      </c>
+      <c r="AI13" s="12"/>
       <c r="AJ13" s="12"/>
-      <c r="AK13" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="AK13" s="12"/>
       <c r="AL13" s="12"/>
-      <c r="AM13" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="AM13" s="12"/>
       <c r="AN13" s="12"/>
       <c r="AP13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ13" s="12" t="s">
-        <v>47</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="AQ13" s="12"/>
       <c r="AR13" s="12"/>
-      <c r="AS13" s="12" t="s">
-        <v>48</v>
-      </c>
+      <c r="AS13" s="12"/>
       <c r="AT13" s="12"/>
-      <c r="AU13" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="AU13" s="12"/>
       <c r="AV13" s="12"/>
-      <c r="AW13" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="AW13" s="12"/>
       <c r="AX13" s="12"/>
       <c r="AZ13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="BA13" s="12" t="s">
-        <v>47</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="BA13" s="12"/>
       <c r="BB13" s="12"/>
-      <c r="BC13" s="12" t="s">
-        <v>48</v>
-      </c>
+      <c r="BC13" s="12"/>
       <c r="BD13" s="12"/>
-      <c r="BE13" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="BE13" s="12"/>
       <c r="BF13" s="12"/>
-      <c r="BG13" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="BG13" s="12"/>
       <c r="BH13" s="12"/>
       <c r="BJ13" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="BK13" s="53">
         <v>0</v>
@@ -2867,7 +2711,7 @@
       <c r="BU13" s="12"/>
       <c r="BV13" s="12"/>
       <c r="BX13" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="BY13" s="52">
         <v>0</v>
@@ -2894,25 +2738,25 @@
       <c r="CI13" s="12"/>
       <c r="CJ13" s="12"/>
       <c r="CL13" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="CM13" s="52">
         <v>89304.508186784</v>
       </c>
       <c r="CN13" s="52">
-        <v>0.06316745688263</v>
+        <v>6.316745688263</v>
       </c>
       <c r="CO13" s="52">
         <v>636093.13683536</v>
       </c>
       <c r="CP13" s="52">
-        <v>0.20832951621092</v>
+        <v>20.832951621092</v>
       </c>
       <c r="CQ13" s="52">
         <v>712744.7578636</v>
       </c>
       <c r="CR13" s="52">
-        <v>0.15955506427662</v>
+        <v>15.955506427662</v>
       </c>
       <c r="CS13" s="12"/>
       <c r="CT13" s="12"/>
@@ -2921,7 +2765,7 @@
       <c r="CW13" s="12"/>
       <c r="CX13" s="12"/>
       <c r="CZ13" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="DA13" s="52">
         <v>0</v>
@@ -2950,7 +2794,7 @@
     </row>
     <row r="14" spans="1:116">
       <c r="B14" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C14" s="52">
         <v>0</v>
@@ -2977,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="M14" s="52">
         <v>0</v>
@@ -3004,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="W14" s="52">
         <v>0</v>
@@ -3031,64 +2875,40 @@
         <v>0</v>
       </c>
       <c r="AF14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG14" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="AG14" s="12"/>
       <c r="AH14" s="12"/>
-      <c r="AI14" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="AI14" s="12"/>
       <c r="AJ14" s="12"/>
-      <c r="AK14" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="AK14" s="12"/>
       <c r="AL14" s="12"/>
-      <c r="AM14" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="AM14" s="12"/>
       <c r="AN14" s="12"/>
       <c r="AP14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ14" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="AQ14" s="12"/>
       <c r="AR14" s="12"/>
-      <c r="AS14" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="AS14" s="12"/>
       <c r="AT14" s="12"/>
-      <c r="AU14" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="AU14" s="12"/>
       <c r="AV14" s="12"/>
-      <c r="AW14" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="AW14" s="12"/>
       <c r="AX14" s="12"/>
       <c r="AZ14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA14" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="BA14" s="12"/>
       <c r="BB14" s="12"/>
-      <c r="BC14" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="BC14" s="12"/>
       <c r="BD14" s="12"/>
-      <c r="BE14" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="BE14" s="12"/>
       <c r="BF14" s="12"/>
-      <c r="BG14" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="BG14" s="12"/>
       <c r="BH14" s="12"/>
       <c r="BJ14" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="BK14" s="53">
         <v>0</v>
@@ -3115,7 +2935,7 @@
       <c r="BU14" s="12"/>
       <c r="BV14" s="12"/>
       <c r="BX14" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="BY14" s="52">
         <v>0</v>
@@ -3142,7 +2962,7 @@
       <c r="CI14" s="12"/>
       <c r="CJ14" s="12"/>
       <c r="CL14" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="CM14" s="31"/>
       <c r="CN14" s="10"/>
@@ -3157,7 +2977,7 @@
       <c r="CW14" s="10"/>
       <c r="CX14" s="11"/>
       <c r="CZ14" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="DA14" s="52">
         <v>0</v>
@@ -3190,117 +3010,117 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="G15" s="30"/>
       <c r="H15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="L15" s="30" t="s">
         <v>27</v>
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="O15" s="30"/>
       <c r="P15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="Q15" s="30"/>
       <c r="R15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="S15" s="30"/>
       <c r="T15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="V15" s="30" t="s">
         <v>27</v>
       </c>
       <c r="W15" s="12"/>
       <c r="X15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="Y15" s="30"/>
       <c r="Z15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AA15" s="30"/>
       <c r="AB15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AC15" s="30"/>
       <c r="AD15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AF15" s="30" t="s">
         <v>27</v>
       </c>
       <c r="AG15" s="12"/>
       <c r="AH15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AI15" s="30"/>
       <c r="AJ15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AK15" s="30"/>
       <c r="AL15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AM15" s="30"/>
       <c r="AN15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AP15" s="30" t="s">
         <v>27</v>
       </c>
       <c r="AQ15" s="12"/>
       <c r="AR15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AS15" s="30"/>
       <c r="AT15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AU15" s="30"/>
       <c r="AV15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AW15" s="30"/>
       <c r="AX15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="AZ15" s="30" t="s">
         <v>27</v>
       </c>
       <c r="BA15" s="12"/>
       <c r="BB15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="BC15" s="30"/>
       <c r="BD15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="BE15" s="30"/>
       <c r="BF15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="BG15" s="30"/>
       <c r="BH15" s="30" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="BJ15" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="BK15" s="53">
         <v>0</v>
@@ -3327,7 +3147,7 @@
       <c r="BU15" s="12"/>
       <c r="BV15" s="12"/>
       <c r="BX15" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="BY15" s="52">
         <v>0</v>
@@ -3354,25 +3174,25 @@
       <c r="CI15" s="12"/>
       <c r="CJ15" s="12"/>
       <c r="CL15" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="CM15" s="52">
         <v>18527.416490214</v>
       </c>
       <c r="CN15" s="52">
-        <v>0.013104935081713</v>
+        <v>1.3104935081713</v>
       </c>
       <c r="CO15" s="52">
         <v>82718.462884909</v>
       </c>
       <c r="CP15" s="52">
-        <v>0.027091468774933</v>
+        <v>2.7091468774933</v>
       </c>
       <c r="CQ15" s="52">
         <v>100026.75894256</v>
       </c>
       <c r="CR15" s="52">
-        <v>0.022391993454011</v>
+        <v>2.2391993454011</v>
       </c>
       <c r="CS15" s="12"/>
       <c r="CT15" s="12"/>
@@ -3381,7 +3201,7 @@
       <c r="CW15" s="12"/>
       <c r="CX15" s="12"/>
       <c r="CZ15" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="DA15" s="52">
         <v>0</v>
@@ -3410,25 +3230,25 @@
     </row>
     <row r="16" spans="1:116">
       <c r="CL16" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="CM16" s="52">
         <v>37067.727812079</v>
       </c>
       <c r="CN16" s="52">
-        <v>0.026218991021252</v>
+        <v>2.6218991021252</v>
       </c>
       <c r="CO16" s="52">
         <v>117635.82958989</v>
       </c>
       <c r="CP16" s="52">
-        <v>0.03852740117502</v>
+        <v>3.852740117502</v>
       </c>
       <c r="CQ16" s="52">
         <v>153630.7087148</v>
       </c>
       <c r="CR16" s="52">
-        <v>0.034391775363354</v>
+        <v>3.4391775363354</v>
       </c>
       <c r="CS16" s="12"/>
       <c r="CT16" s="12"/>
@@ -3439,7 +3259,7 @@
     </row>
     <row r="17" spans="1:116">
       <c r="CL17" s="9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="CM17" s="31"/>
       <c r="CN17" s="10"/>
@@ -3456,7 +3276,7 @@
     </row>
     <row r="18" spans="1:116">
       <c r="CL18" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="CM18" s="52">
         <v>0</v>
@@ -3498,7 +3318,7 @@
       <c r="CI19" s="14"/>
       <c r="CJ19" s="14"/>
       <c r="CL19" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="CM19" s="52">
         <v>0</v>
@@ -3510,13 +3330,13 @@
         <v>1837.2526066584</v>
       </c>
       <c r="CP19" s="52">
-        <v>0.00060172626387176</v>
+        <v>0.060172626387176</v>
       </c>
       <c r="CQ19" s="52">
         <v>1784.8038156153</v>
       </c>
       <c r="CR19" s="52">
-        <v>0.00039954623921085</v>
+        <v>0.039954623921085</v>
       </c>
       <c r="CS19" s="12"/>
       <c r="CT19" s="12"/>
@@ -3540,7 +3360,7 @@
       <c r="CI20" s="14"/>
       <c r="CJ20" s="14"/>
       <c r="CL20" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="CM20" s="31"/>
       <c r="CN20" s="10"/>
@@ -3571,7 +3391,7 @@
       <c r="CJ21" s="2"/>
       <c r="CK21" s="21"/>
       <c r="CL21" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="CM21" s="52">
         <v>0</v>
@@ -3614,7 +3434,7 @@
       <c r="CJ22" s="2"/>
       <c r="CK22" s="21"/>
       <c r="CL22" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="CM22" s="52">
         <v>0</v>
@@ -3656,7 +3476,7 @@
       <c r="CI23" s="1"/>
       <c r="CJ23" s="5"/>
       <c r="CL23" s="9" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="CM23" s="31"/>
       <c r="CN23" s="10"/>
@@ -3686,7 +3506,7 @@
       <c r="CI24" s="14"/>
       <c r="CJ24" s="14"/>
       <c r="CL24" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="CM24" s="52">
         <v>0</v>
@@ -3728,7 +3548,7 @@
       <c r="CI25" s="14"/>
       <c r="CJ25" s="14"/>
       <c r="CL25" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="CM25" s="52">
         <v>0</v>

</xml_diff>